<commit_message>
fix free shipping limit
</commit_message>
<xml_diff>
--- a/public/assets/xls/plava-krava.xlsx
+++ b/public/assets/xls/plava-krava.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>products(3)</t>
   </si>
@@ -98,54 +98,25 @@
     <t>Povezani proizvodi</t>
   </si>
   <si>
-    <t>Michael Scott</t>
-  </si>
-  <si>
-    <t>Plava Krava</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alkemičar 
-</t>
-  </si>
-  <si>
-    <t>PK40</t>
-  </si>
-  <si>
-    <t>On čuva tajnu koja može značiti kraj svijeta. Istina: Nicholas Flamel rođen je 28. rujna 1330. godine u Parizu. Gotovo sedamsto godina kasnije još ga uvijek prati glas najvećeg alkemičara njegova doba. Priča se da spoznao tajnu vječnoga života. Svi spisi navode da je umro 1418. godine. Njegova je grobnica, međutim, prazna. Legenda: Nicholas Flamel je živ. No samo zahvaljujući eliksiru života što ga proizvodi već stoljećima. Tajna besmrtnosti skrivena je u Knjizi Abrahama Židova. Upadne li ta knjiga u krive ruke, svijet će biti uništen. Upravo je to ono čemu se doktor John Dee nada i što planira učiniti čim se knjige dokopa. Ljudski rod pojma neće imati što se događa sve dok ne budem prekasno. A ako je vjerovati proročanstvu, jedini u čijoj je moći da svijet spase od potpuna uništenja su blizanci Sophie i Josh Newman. Ponekad se legende obistine. A Sophie i Josh Newman naći će se usred jedne od najvećih legendi svih vremena. Iz pera neupitnog autoriteta s područja mitologije i folkloristike, Michaela Scotta, majstora fantastike i jednog od najuspješnijih suvremenih irskih pisaca, predstavljamo još jedan od od najljepših izdanaka svjetske književnosti za mlade. Prije svega čarobnu, nesvakidašnju priču o hrabrosti i odanosti na hrvatskome je ispripovjedila Marija Kostović, a naslovna ilustracija,preuzeta s originalnog izdanja, djelo je Michaela Wagnera.</t>
-  </si>
-  <si>
-    <t>alkemicar-michael-scott</t>
-  </si>
-  <si>
-    <t>Beletristika, Fantazija, Immortal, Knjige</t>
-  </si>
-  <si>
-    <t>26.41</t>
-  </si>
-  <si>
-    <t>22.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alkemičar – Michael Scott 
-</t>
-  </si>
-  <si>
-    <t>Iz pera neupitnog autoriteta s područja mitologije i folkloristike, Michaela Scotta, majstora fantastike i jednog od najuspješnijih suvremenih irskih pisaca, predstavljamo još jedan od od najljepših izdanaka svjetske književnosti za mlade.</t>
-  </si>
-  <si>
-    <t>15x24.5</t>
-  </si>
-  <si>
-    <t>Zagreb</t>
-  </si>
-  <si>
-    <t>Latinica</t>
-  </si>
-  <si>
-    <t>Tvrdi</t>
-  </si>
-  <si>
-    <t>Hrvatski</t>
+    <t>Džo Elen Mur</t>
+  </si>
+  <si>
+    <t>Delfi</t>
+  </si>
+  <si>
+    <t>Vežbam kod kuće 1 - Matematika</t>
+  </si>
+  <si>
+    <t>A287148</t>
+  </si>
+  <si>
+    <t>10,1010256410256</t>
+  </si>
+  <si>
+    <t>Ćirilica</t>
+  </si>
+  <si>
+    <t>Srpski</t>
   </si>
   <si>
     <t>Attribute</t>
@@ -182,7 +153,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -203,6 +174,11 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -330,6 +306,51 @@
       </right>
       <top style="thin">
         <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -423,58 +444,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -493,25 +469,40 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -520,6 +511,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
@@ -538,19 +532,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -802,7 +790,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -832,7 +819,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -858,7 +844,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -884,7 +869,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -910,7 +894,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -936,7 +919,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -962,7 +944,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -988,7 +969,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1014,7 +994,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1040,7 +1019,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1091,7 +1069,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1117,7 +1094,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1143,7 +1119,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1169,7 +1144,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1195,7 +1169,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1221,7 +1194,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1247,7 +1219,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1273,7 +1244,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1299,7 +1269,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1325,7 +1294,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1373,7 +1341,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1403,7 +1370,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1429,7 +1395,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1455,7 +1420,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1481,7 +1445,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1507,7 +1470,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1533,7 +1495,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1559,7 +1520,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1585,7 +1545,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1611,7 +1570,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1640,7 +1598,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1649,14 +1607,14 @@
     <col min="1" max="1" width="3.35156" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.3203" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3516" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.1719" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.35156" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.2969" style="1" customWidth="1"/>
     <col min="8" max="8" width="52" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.5469" style="1" customWidth="1"/>
-    <col min="10" max="10" width="32.6094" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.2891" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="32.6719" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.3516" style="1" customWidth="1"/>
     <col min="12" max="12" width="15.1719" style="1" customWidth="1"/>
     <col min="13" max="13" width="7.85156" style="1" customWidth="1"/>
     <col min="14" max="14" width="17" style="1" customWidth="1"/>
@@ -1788,10 +1746,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" ht="68.65" customHeight="1">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
+    <row r="3" ht="14.7" customHeight="1">
+      <c r="A3" s="6"/>
       <c r="B3" t="s" s="7">
         <v>28</v>
       </c>
@@ -1804,240 +1760,40 @@
       <c r="E3" t="s" s="8">
         <v>31</v>
       </c>
-      <c r="F3" s="10">
-        <v>6</v>
-      </c>
-      <c r="G3" s="11"/>
-      <c r="H3" t="s" s="8">
+      <c r="F3" s="10"/>
+      <c r="G3" s="11">
+        <v>9788652912575</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" t="s" s="12">
         <v>32</v>
       </c>
-      <c r="I3" t="s" s="8">
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" t="s" s="12">
         <v>33</v>
       </c>
-      <c r="J3" t="s" s="8">
+      <c r="V3" s="8"/>
+      <c r="W3" s="10"/>
+      <c r="X3" t="s" s="8">
         <v>34</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="M3" s="10">
-        <v>203</v>
-      </c>
-      <c r="N3" s="10">
-        <v>5</v>
-      </c>
-      <c r="O3" t="s" s="8">
-        <v>36</v>
-      </c>
-      <c r="P3" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="Q3" t="s" s="8">
-        <v>38</v>
-      </c>
-      <c r="R3" s="10">
-        <v>268</v>
-      </c>
-      <c r="S3" t="s" s="8">
-        <v>39</v>
-      </c>
-      <c r="T3" t="s" s="8">
-        <v>40</v>
-      </c>
-      <c r="U3" t="s" s="8">
-        <v>41</v>
-      </c>
-      <c r="V3" t="s" s="8">
-        <v>42</v>
-      </c>
-      <c r="W3" s="10">
-        <v>2021</v>
-      </c>
-      <c r="X3" t="s" s="8">
-        <v>43</v>
-      </c>
-      <c r="Y3" s="10">
-        <v>9789538420214</v>
-      </c>
-      <c r="Z3" s="10">
-        <v>1</v>
+      <c r="Y3" s="11">
+        <v>9788652912575</v>
+      </c>
+      <c r="Z3" s="13">
+        <v>0</v>
       </c>
       <c r="AA3" s="8"/>
-    </row>
-    <row r="4" ht="14.7" customHeight="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13"/>
-      <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="14"/>
-    </row>
-    <row r="5" ht="14.7" customHeight="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
-      <c r="AA5" s="17"/>
-    </row>
-    <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="17"/>
-    </row>
-    <row r="7" ht="14.7" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="17"/>
-    </row>
-    <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="17"/>
-    </row>
-    <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="19"/>
-      <c r="X9" s="19"/>
-      <c r="Y9" s="19"/>
-      <c r="Z9" s="19"/>
-      <c r="AA9" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2062,37 +1818,37 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="21" customWidth="1"/>
-    <col min="2" max="2" width="36" style="21" customWidth="1"/>
-    <col min="3" max="3" width="28.3516" style="21" customWidth="1"/>
-    <col min="4" max="4" width="31.6719" style="21" customWidth="1"/>
-    <col min="5" max="5" width="27.3516" style="21" customWidth="1"/>
-    <col min="6" max="6" width="30.5" style="21" customWidth="1"/>
-    <col min="7" max="7" width="25.3516" style="21" customWidth="1"/>
-    <col min="8" max="8" width="52" style="21" customWidth="1"/>
-    <col min="9" max="9" width="43.6719" style="21" customWidth="1"/>
-    <col min="10" max="10" width="48.8516" style="21" customWidth="1"/>
-    <col min="11" max="11" width="62.3516" style="21" customWidth="1"/>
-    <col min="12" max="12" width="15.1719" style="21" customWidth="1"/>
-    <col min="13" max="13" width="7.85156" style="21" customWidth="1"/>
-    <col min="14" max="14" width="17" style="21" customWidth="1"/>
-    <col min="15" max="15" width="12.8516" style="21" customWidth="1"/>
-    <col min="16" max="17" width="45.8516" style="21" customWidth="1"/>
-    <col min="18" max="18" width="19.5" style="21" customWidth="1"/>
-    <col min="19" max="19" width="13.6719" style="21" customWidth="1"/>
-    <col min="20" max="20" width="16.5" style="21" customWidth="1"/>
-    <col min="21" max="21" width="13" style="21" customWidth="1"/>
-    <col min="22" max="22" width="12.3516" style="21" customWidth="1"/>
-    <col min="23" max="23" width="11" style="21" customWidth="1"/>
-    <col min="24" max="25" width="17.3516" style="21" customWidth="1"/>
-    <col min="26" max="26" width="18.6719" style="21" customWidth="1"/>
-    <col min="27" max="27" width="27.3516" style="21" customWidth="1"/>
-    <col min="28" max="16384" width="8.35156" style="21" customWidth="1"/>
+    <col min="1" max="1" width="18.5" style="14" customWidth="1"/>
+    <col min="2" max="2" width="36" style="14" customWidth="1"/>
+    <col min="3" max="3" width="28.3516" style="14" customWidth="1"/>
+    <col min="4" max="4" width="31.6719" style="14" customWidth="1"/>
+    <col min="5" max="5" width="27.3516" style="14" customWidth="1"/>
+    <col min="6" max="6" width="30.5" style="14" customWidth="1"/>
+    <col min="7" max="7" width="25.3516" style="14" customWidth="1"/>
+    <col min="8" max="8" width="52" style="14" customWidth="1"/>
+    <col min="9" max="9" width="43.6719" style="14" customWidth="1"/>
+    <col min="10" max="10" width="48.8516" style="14" customWidth="1"/>
+    <col min="11" max="11" width="62.3516" style="14" customWidth="1"/>
+    <col min="12" max="12" width="15.1719" style="14" customWidth="1"/>
+    <col min="13" max="13" width="7.85156" style="14" customWidth="1"/>
+    <col min="14" max="14" width="17" style="14" customWidth="1"/>
+    <col min="15" max="15" width="12.8516" style="14" customWidth="1"/>
+    <col min="16" max="17" width="45.8516" style="14" customWidth="1"/>
+    <col min="18" max="18" width="19.5" style="14" customWidth="1"/>
+    <col min="19" max="19" width="13.6719" style="14" customWidth="1"/>
+    <col min="20" max="20" width="16.5" style="14" customWidth="1"/>
+    <col min="21" max="21" width="13" style="14" customWidth="1"/>
+    <col min="22" max="22" width="12.3516" style="14" customWidth="1"/>
+    <col min="23" max="23" width="11" style="14" customWidth="1"/>
+    <col min="24" max="25" width="17.3516" style="14" customWidth="1"/>
+    <col min="26" max="26" width="18.6719" style="14" customWidth="1"/>
+    <col min="27" max="27" width="27.3516" style="14" customWidth="1"/>
+    <col min="28" max="16384" width="8.35156" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2126,25 +1882,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s" s="5">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s" s="5">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s" s="5">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s" s="5">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s" s="5">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -2167,240 +1923,240 @@
       <c r="AA2" s="5"/>
     </row>
     <row r="3" ht="68.65" customHeight="1">
-      <c r="A3" s="6">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="8"/>
       <c r="D3" s="9"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
       <c r="O3" s="8"/>
       <c r="P3" s="9"/>
       <c r="Q3" s="8"/>
-      <c r="R3" s="11"/>
+      <c r="R3" s="10"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
-      <c r="W3" s="11"/>
+      <c r="W3" s="10"/>
       <c r="X3" s="8"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" t="s" s="25">
-        <v>52</v>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" t="s" s="20">
+        <v>43</v>
       </c>
     </row>
     <row r="5" ht="14.7" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="14"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="23"/>
     </row>
     <row r="6" ht="14.7" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="17"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="26"/>
     </row>
     <row r="7" ht="14.7" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="17"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="25"/>
+      <c r="AA7" s="26"/>
     </row>
     <row r="8" ht="14.7" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="17"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+      <c r="Y8" s="25"/>
+      <c r="Z8" s="25"/>
+      <c r="AA8" s="26"/>
     </row>
     <row r="9" ht="14.7" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="17"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="26"/>
     </row>
     <row r="10" ht="14.7" customHeight="1">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="19"/>
-      <c r="AA10" s="20"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>